<commit_message>
Harry | Minor updates
</commit_message>
<xml_diff>
--- a/src/main/resources/data/Testdata.xlsx
+++ b/src/main/resources/data/Testdata.xlsx
@@ -80,10 +80,10 @@
     <t>DXB</t>
   </si>
   <si>
-    <t>2872023</t>
-  </si>
-  <si>
-    <t>2082023</t>
+    <t>11X2023</t>
+  </si>
+  <si>
+    <t>20X2023</t>
   </si>
   <si>
     <t>2</t>
@@ -98,10 +98,10 @@
     <t>Search Flight_002</t>
   </si>
   <si>
-    <t>2972024</t>
-  </si>
-  <si>
-    <t>1282023</t>
+    <t>10X2023</t>
+  </si>
+  <si>
+    <t>12X2023</t>
   </si>
 </sst>
 </file>

</xml_diff>